<commit_message>
✨ Ready for Render deployment
</commit_message>
<xml_diff>
--- a/emails_generes.xlsx
+++ b/emails_generes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,30 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CIC</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Erreur : 502 Server Error: Bad Gateway for url: https://chatbot-o4gm.onrender.com/generate_email</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Claire Huteau</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Erreur : 502 Server Error: Bad Gateway for url: https://chatbot-o4gm.onrender.com/generate_email</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Déploiement initial du bot Telegram sur Render
</commit_message>
<xml_diff>
--- a/emails_generes.xlsx
+++ b/emails_generes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,36 +448,1174 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Anne CUMIN</t>
+          <t>Campus The Land Rennes</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Erreur : 503 Server Error: Service Unavailable for url: https://chatbot-o4gm.onrender.com/generate_email</t>
+          <t>Madame, Monsieur,
+J'ai récemment visité votre site web et j'ai été impressionné par la diversité des activités proposées au Campus The Land Rennes. Votre engagement envers l'éducation et le développement des étudiants est admirable.
+Je pense que la création de vidéos personnalisées pourrait être un excellent moyen de mettre en lumière vos programmes et vos valeurs. Nous pourrions envisager un format de reportage pour mettre en avant l'immersion dans votre campus ou une série de vidéos pour présenter vos différents cursus de manière dynamique.
+Une collaboration vidéo avec La Station vous permettrait d'accroître votre visibilité en ligne, de renforcer votre crédibilité auprès de vos futurs étudiants et partenaires, tout en véhiculant vos valeurs et votre engagement.
+Je vous propose de discuter plus en détail de cette opportunité lors d'un rendez-vous rapide. Seriez-vous disponible pour un appel la semaine prochaine ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel
+La Station
+contact@lastation-prod.com
+06 75 61 11 72
+www.lastation-prod.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CIC</t>
+          <t>CABEC</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Erreur : 502 Server Error: Bad Gateway for url: https://chatbot-o4gm.onrender.com/generate_email</t>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre entreprise CABEC et je suis impressionné par votre engagement à accompagner les entrepreneurs dans leur développement. Votre approche personnalisée et de qualité correspond parfaitement à nos valeurs chez La Station.
+Je suis convaincu que la création de vidéos personnalisées pourrait grandement contribuer à renforcer votre visibilité et votre crédibilité auprès de vos clients et partenaires. Nous pourrions par exemple envisager la réalisation d'un film d'entreprise mettant en avant vos services de manière authentique et engageante.
+De plus, un témoignage vidéo de vos clients actuels pourrait renforcer la confiance de vos prospects et mettre en lumière la qualité de vos services. Ces formats vidéos pourraient véhiculer vos valeurs et votre professionnalisme de manière percutante.
+Je serais ravi de discuter plus en détail de ces possibilités lors d'un rendez-vous téléphonique rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Claire Huteau</t>
+          <t>KINGYO -food truck japonais-</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Erreur : 502 Server Error: Bad Gateway for url: https://chatbot-o4gm.onrender.com/generate_email</t>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre food truck japonais, Kingyo, et je suis impressionné par la qualité de vos plats et l'authenticité de votre cuisine. Votre concept de food truck itinérant qui propose des plats traditionnels japonais revisités est vraiment original et séduisant.
+Je pense que la création de vidéos personnalisées pourrait être un excellent moyen de mettre en valeur votre entreprise et de partager votre passion pour la cuisine japonaise avec un public plus large. Un format de reportage ou une publicité mettant en avant l'immersion dans votre activité et le fort impact de vos plats pourraient vraiment renforcer votre visibilité et votre notoriété.
+En collaborant avec La Station, nous pourrions vous aider à transmettre vos valeurs, à renforcer votre crédibilité et à susciter l'intérêt de nouveaux clients. Nous serions ravis de discuter plus en détail de la manière dont nous pourrions travailler ensemble pour créer des contenus vidéo originaux et impactants pour Kingyo.
+Je vous propose de convenir d'un rendez-vous téléphonique rapide pour échanger sur vos besoins et vos attentes en matière de communication vidéo. N'hésitez pas à me contacter par email ou par téléphone pour fixer un créneau qui vous conviendrait.
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Natixis</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à ma découverte de votre entreprise Natixis, spécialisée dans l'épargne salariale et retraite. Vos valeurs et votre position de leader dans le domaine m'ont particulièrement interpellé.
+Je suis Alan Roussel, expert en prospection B2B pour l'agence rennaise La Station, spécialisée dans la création de vidéos personnalisées. Nous proposons des formats vidéo tels que des interviews, des reportages ou des publicités, qui pourraient parfaitement mettre en valeur votre expertise et vos services.
+Une collaboration avec La Station vous permettrait de renforcer votre visibilité, de transmettre vos valeurs de manière authentique et de gagner en crédibilité auprès de votre audience.
+Je vous propose un échange rapide pour discuter des possibilités de collaboration et des bénéfices que des vidéos personnalisées pourraient apporter à Natixis.
+Dans l'attente de votre retour, je vous propose de convenir d'un rendez-vous téléphonique à votre convenance.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Espace France services de Romillé</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter au sujet de votre Espace France Services de Romillé. En tant qu'agence spécialisée dans la création de vidéos personnalisées, nous sommes convaincus que la vidéo pourrait être un outil efficace pour mettre en avant les services que vous proposez.
+Avez-vous déjà envisagé de réaliser des témoignages de vos utilisateurs pour illustrer l'impact de votre Espace France Services ? Ou peut-être une vidéo de présentation pour faciliter l'accès aux droits que vous offrez ?
+Nous sommes convaincus que la vidéo pourrait renforcer la visibilité de votre structure, mettre en avant vos valeurs d'entraide et de proximité, et renforcer votre crédibilité auprès de vos usagers.
+Serait-il possible d'échanger rapidement sur ces idées et de discuter des possibilités de collaboration vidéo ? Un appel téléphonique pourrait être l'occasion parfaite pour en discuter plus en détail.
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Justine Guinet</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre entreprise, l'Office Notarial de Justine Guinet, et je suis impressionné par vos valeurs et votre expertise dans le domaine du notariat. 
+Je suis Alan Roussel, expert en prospection B2B pour l'agence audiovisuelle La Station à Rennes. Nous sommes spécialisés dans la création de vidéos personnalisées pour les entreprises, et je pense que notre collaboration pourrait vous apporter une réelle valeur ajoutée.
+Je vous propose de discuter des possibilités de réaliser un film d'entreprise mettant en avant vos savoir-faire spécialisés et votre équipe humaine. Ce format vidéo pourrait renforcer votre visibilité en ligne et mettre en lumière les services uniques que vous proposez à vos clients.
+Si cette proposition vous intéresse, je serais ravi de convenir d'un rendez-vous rapide pour discuter plus en détail de vos besoins et de nos solutions vidéo sur mesure.
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>GAUMER Associés expert-comptable</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à ma découverte de votre entreprise GAUMER Associés expert-comptable. Votre engagement à garantir le respect des obligations légales de vos clients en matière de comptabilité et de fiscalité est admirable.
+Je suis Alan Roussel, expert en prospection B2B pour l'agence La Station, spécialisée dans la création de vidéos personnalisées. Je pense que la réalisation d'un film d'entreprise ou d'une interview pourrait grandement valoriser votre expertise et renforcer la confiance de vos clients actuels et futurs.
+En mettant en avant vos valeurs et votre proximité avec vos clients à travers une vidéo, vous pourriez accroître votre visibilité et renforcer votre crédibilité sur le marché. 
+Je serais ravi de discuter plus en détail de cette opportunité lors d'un rendez-vous téléphonique rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>St Bernard PC</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car je suis tombé sur votre site web et j'ai été impressionné par votre approche innovante en matière de dépannage informatique à domicile, notamment en cette période de Covid19.
+Je pense que la création d'une vidéo personnalisée pourrait grandement renforcer votre communication et mettre en avant les valeurs de St Bernard PC. Que diriez-vous d'un film d'entreprise mettant en lumière votre engagement envers la sécurité de vos clients, ou d'un reportage captivant montrant votre équipe en action tout en respectant les gestes barrières ?
+Une vidéo bien réalisée peut non seulement renforcer votre visibilité en ligne, mais aussi renforcer la confiance de vos clients en mettant en avant votre professionnalisme et votre souci du détail.
+Je serais ravi de discuter de ces idées plus en détail lors d'un rendez-vous téléphonique rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Penny Lane</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Madame, Monsieur,
+J'ai récemment découvert votre établissement Penny Lane à Rennes et j'ai été impressionné par l'ambiance chaleureuse que vous semblez offrir à vos clients. Votre présence sur les réseaux sociaux, notamment sur Facebook, montre une belle dynamique et une proximité avec votre communauté.
+Je me permets de vous contacter car je pense que la création de vidéos personnalisées pourrait être un atout majeur pour mettre en avant l'expérience unique que vous proposez à vos clients. Un format d'aftermovie captivant pourrait parfaitement retranscrire l'ambiance de votre bar et susciter l'intérêt de nouveaux clients en quête de lieux authentiques.
+En collaborant avec La Station, vous pourriez renforcer votre visibilité en ligne, valoriser vos valeurs d'authenticité et de convivialité, et renforcer votre crédibilité auprès de votre audience.
+Je vous propose un échange rapide pour discuter de vos besoins en matière de communication vidéo et explorer les possibilités de collaboration. Seriez-vous disponible pour un rendez-vous téléphonique cette semaine ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel
+La Station
+contact@lastation-prod.com
+06 75 61 11 72
+www.lastation-prod.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>WILLY KS Company</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre entreprise, Willy KS Company, spécialisée dans l'import-export de fruits et légumes exotiques, et j'ai été impressionné par votre engagement envers la qualité et l'origine de vos produits.
+Je suis Alan Roussel, expert en prospection B2B pour l'agence La Station à Rennes. Nous sommes spécialisés dans la création de vidéos personnalisées pour les entreprises, et je pense que notre expertise pourrait vous aider à mettre en avant la qualité de vos produits et l'engagement de votre entreprise.
+Je vous propose de discuter des possibilités de collaboration pour la création d'un film d'entreprise mettant en valeur vos produits phares comme le KENT Mango et l'avocat premium. Une vidéo authentique et dynamique pourrait renforcer votre visibilité et votre crédibilité auprès de vos clients actuels et futurs.
+Serait-il possible de convenir d'un rendez-vous rapide pour discuter de cette opportunité ? Je suis convaincu que notre collaboration pourrait être bénéfique pour votre entreprise.
+Je vous remercie pour votre attention et reste à votre disposition pour toute question ou information supplémentaire.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Rousseau Confort Et Services</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment visité votre site web et j'ai été impressionné par la qualité de vos services de confort et de services à domicile. Votre engagement envers la satisfaction de vos clients est admirable.
+Je pense que la création de vidéos personnalisées pourrait être un excellent moyen de mettre en avant votre entreprise et de renforcer votre présence en ligne. Plus particulièrement, un reportage immersif sur vos activités ou une publicité percutante pour mettre en avant vos services pourraient véritablement vous aider à toucher un public plus large et à renforcer votre image de marque.
+En collaborant avec La Station, vous pourriez bénéficier d'une visibilité accrue, d'une mise en valeur de vos valeurs et de votre professionnalisme, ainsi que d'une crédibilité renforcée auprès de vos clients actuels et potentiels.
+Je serais ravi de discuter de ces opportunités de collaboration plus en détail lors d'un rendez-vous ou d'un appel rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Talents Croisés</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à la découverte de votre entreprise Talents Croisés. Votre approche humaine et votre engagement envers vos clients et talents sont des valeurs qui résonnent fortement avec notre vision chez La Station.
+Je suis impressionné par votre expertise dans les secteurs banque, assurance et finance, et je suis convaincu que la création de contenus vidéo personnalisés pourrait grandement renforcer votre communication et votre image de marque. 
+Je vous propose de discuter des possibilités de collaboration pour la réalisation de films d'entreprise mettant en avant vos valeurs et votre expertise, ou bien des témoignages clients pour renforcer votre crédibilité et votre visibilité.
+Une vidéo personnalisée pourrait véhiculer vos messages de manière impactante et toucher un public plus large, renforçant ainsi votre position sur le marché.
+Serait-il possible d'échanger rapidement sur ces opportunités ? Un rendez-vous téléphonique pourrait être l'occasion parfaite pour discuter plus en détail.
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Denis Riou</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre site web et je suis impressionné par la qualité de vos photographies. Votre expertise en tant que photographe professionnel depuis plus de 35 ans est indéniable.
+Je me permets de vous contacter car je pense que la vidéo pourrait être un excellent moyen de mettre en valeur votre travail et d'atteindre un public plus large. Nous pourrions envisager de réaliser un film promotionnel mettant en lumière votre approche artistique ou des témoignages de clients satisfaits pour renforcer votre crédibilité.
+Une vidéo bien réalisée pourrait non seulement augmenter votre visibilité en ligne, mais aussi renforcer les valeurs que vous véhiculez à travers votre travail.
+Je serais ravi de discuter de cette opportunité de collaboration avec vous. Seriez-vous disponible pour un rendez-vous rapide afin d'échanger plus en détail sur vos besoins et attentes en matière de contenu vidéo ?
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Isabelle Lechevallier Photographe</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je suis Alan Roussel, expert en prospection B2B pour l'agence rennaise La Station, spécialisée dans la création de vidéos personnalisées. En visitant votre site web, j'ai été impressionné par la qualité de vos services de photographie et votre dévouement à capturer les moments précieux de la vie de vos clients.
+Je pense que la vidéo pourrait être un excellent complément à votre offre actuelle. Imaginez des témoignages vidéo de vos clients satisfaits partageant leurs expériences, ou des reportages capturant l'émotion et la beauté de vos séances photo. Ces formats pourraient renforcer votre visibilité en ligne et mettre en avant vos valeurs d'authenticité et de professionnalisme.
+Je serais ravi de discuter plus en détail de la manière dont La Station pourrait vous accompagner dans la création de contenus vidéo uniques et impactants. Seriez-vous disponible pour un appel rapide cette semaine pour échanger sur les possibilités de collaboration ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Bechu photographie</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre entreprise Bechu Photographie et je suis impressionné par la diversité de vos services en matière de photographie. Votre approche sur mesure pour valoriser l'image de vos clients est tout à fait remarquable.
+Je me permets de vous contacter aujourd'hui pour vous proposer une collaboration vidéo avec notre agence La Station. Nous pourrions envisager la réalisation d'un reportage immersif mettant en lumière vos différentes prestations, ou bien d'une série de vidéos de type portrait pour mettre en avant le savoir-faire de votre équipe.
+Une vidéo personnalisée pourrait non seulement renforcer votre visibilité en ligne, mais également véhiculer vos valeurs et renforcer votre crédibilité auprès de vos clients actuels et futurs.
+Je serais ravi de discuter de ces possibilités de collaboration plus en détail lors d'un rendez-vous téléphonique rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Petra Kovacova Photographe</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre site web et j'ai été impressionné par la qualité de vos photographies. Votre approche artistique et naturelle semble parfaitement correspondre à notre expertise en création de vidéos personnalisées.
+Je pense que la réalisation d'un reportage mettant en avant votre travail et votre univers artistique pourrait être un excellent moyen de valoriser votre activité et de renforcer votre présence en ligne. De plus, un aftermovie capturant l'émotion et l'authenticité de vos séances photos pourrait véritablement toucher votre audience et renforcer votre image de marque.
+Nous serions ravis de discuter de ces idées plus en détail lors d'un rendez-vous téléphonique rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel
+La Station
+contact@lastation-prod.com
+06 75 61 11 72
+www.lastation-prod.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Manon Bertho Studio</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre site web, et je suis impressionné par la créativité et la précision qui se dégagent de vos réalisations. Votre univers graphique captivant reflète parfaitement votre engagement à figer des instants et des émotions dans le temps.
+Je me permets de vous contacter aujourd'hui pour vous proposer une collaboration vidéo avec La Station. Nous pourrions envisager la création d'un film d'entreprise mettant en valeur votre savoir-faire et votre personnalité unique, ou bien d'un reportage métier pour montrer l'envers du décor de votre entreprise et mettre en avant votre passion et votre expertise.
+Une vidéo réalisée par nos soins pourrait renforcer votre visibilité en ligne, transmettre vos valeurs de manière authentique et renforcer la crédibilité de votre entreprise auprès de vos clients et partenaires.
+Je serais ravi de pouvoir échanger plus en détail sur les possibilités de collaboration qui s'offrent à nous. Seriez-vous disponible pour un rendez-vous rapide afin d'en discuter de vive voix ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Cabinet Le Guen &amp; Associés</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Madame, Monsieur,
+Je me permets de vous contacter suite à la découverte de votre cabinet Le Guen &amp; Associés, spécialisé dans le conseil en propriété intellectuelle. Votre expertise dans les domaines des Télécoms, de l'Électricité et de l'Électronique, entre autres, m'a particulièrement impressionné.
+Je suis Alan Roussel, expert en prospection B2B pour l'agence rennaise La Station, spécialisée dans la création de vidéos personnalisées. Nous pourrions envisager ensemble la réalisation d'un film d'entreprise mettant en lumière votre savoir-faire et vos valeurs uniques, ou bien d'une interview de vos experts pour renforcer votre crédibilité et votre visibilité.
+Une collaboration vidéo avec La Station pourrait vous permettre de véhiculer efficacement vos messages, de renforcer votre image de marque et d'atteindre de nouveaux clients et partenaires.
+Je vous propose un échange rapide pour discuter de vos besoins et des opportunités de collaboration vidéo. Seriez-vous disponible pour un rendez-vous téléphonique cette semaine ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Piscines Freedom Ouest - Rennes</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à ma découverte de votre entreprise, Piscines Freedom Ouest. Votre expertise dans la conception et l'installation de piscines monocoques en polyester premium sur l'ensemble du Nord-Ouest de la France est impressionnante.
+Je suis Alan Roussel, expert en prospection B2B pour l'agence La Station à Rennes, spécialisée dans la création de vidéos personnalisées. Je pense que la réalisation d'un reportage ou d'une publicité mettant en avant vos réalisations et votre savoir-faire pourrait grandement renforcer votre visibilité et votre crédibilité auprès de vos clients potentiels.
+Nous pourrions travailler ensemble pour capturer de manière authentique et dynamique l'installation de vos piscines, ou créer des vidéos courtes à fort impact mettant en avant le grand choix de couleurs de vos coques, une exclusivité de Freedom Piscines Ouest.
+Je serais ravi de discuter de cette opportunité de collaboration avec vous lors d'un rendez-vous rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Meilleurtaux Placement - Agence de Rennes - Tour d'Auvergne</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter au sujet d'une potentielle collaboration vidéo entre Meilleurtaux Placement et notre agence La Station. En visitant votre site web, j'ai pu constater l'engagement de votre entreprise dans le domaine de la finance et de l'assurance, et je suis convaincu que la création de contenus vidéo originaux pourrait grandement contribuer à renforcer votre présence en ligne.
+Nous proposons une large gamme de formats vidéo adaptés à vos enjeux, tels que des interviews pour mettre en avant vos services, des reportages pour une immersion authentique dans votre activité, ou encore des publicités percutantes pour booster votre visibilité sur les réseaux sociaux.
+Une vidéo personnalisée pourrait non seulement renforcer la crédibilité de Meilleurtaux Placement, mais aussi véhiculer vos valeurs et vous démarquer de la concurrence.
+Je vous propose de discuter plus en détail de vos besoins et attentes lors d'un rendez-vous rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Fortheshoot Production</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à la découverte de votre société Fortheshoot Production, spécialisée dans la production audiovisuelle à Rennes. Votre expertise dans la captation, le tournage et la diffusion de contenus vidéo m'a particulièrement impressionné.
+Je suis convaincu que notre agence La Station pourrait vous accompagner dans la création de vidéos personnalisées pour valoriser vos services et renforcer votre communication. Plus précisément, je pense que notre format d'interview ou de reportage pourrait mettre en lumière vos activités de manière authentique et dynamique, tout en renforçant votre présence en ligne.
+La vidéo est un outil puissant pour accroître la visibilité de votre entreprise, transmettre vos valeurs et renforcer votre crédibilité auprès de vos clients et partenaires. Nous serions ravis de discuter de la manière dont nous pourrions collaborer pour atteindre vos objectifs.
+Je vous propose un échange rapide pour discuter de vos besoins et des possibilités de collaboration. N'hésitez pas à me contacter pour convenir d'un rendez-vous.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>RESO 35 Rennes | Recrutement en Restauration Hôtellerie Tourisme</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre entreprise RESO 35 Rennes spécialisée dans le recrutement en Restauration, Hôtellerie et Tourisme, et je suis impressionné par votre engagement et vos actions dans le secteur. 
+Je pense que la création de vidéos personnalisées pourrait grandement contribuer à mettre en avant vos valeurs et votre expertise. Nous pourrions par exemple réaliser un reportage immersif sur vos activités ou une série de témoignages de vos collaborateurs et partenaires pour renforcer votre visibilité et votre crédibilité.
+Une collaboration vidéo avec La Station pourrait vous permettre de valoriser votre savoir-faire et de toucher un public plus large. 
+Serait-il possible d'échanger rapidement sur les possibilités de collaboration vidéo entre RESO 35 Rennes et La Station ? Un appel serait l'occasion parfaite pour discuter de vos besoins et de nos solutions.
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Unikase Consulting</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+En visitant votre site web, j'ai été impressionné par la clarté de vos valeurs et la pertinence de votre approche envers les PME en phase de croissance. Votre démarche pragmatique et audacieuse correspond parfaitement à notre vision chez La Station.
+Je pense que la création d'un film d'entreprise ou d'une interview personnalisée pourrait grandement renforcer votre communication digitale en mettant en lumière vos expertises et en renforçant votre crédibilité auprès de vos clients et partenaires.
+Grâce à nos services, vous pourriez bénéficier d'une visibilité accrue, d'une mise en valeur de vos valeurs et d'une communication authentique et impactante.
+Je vous propose de discuter de ces opportunités lors d'un rendez-vous rapide. Seriez-vous disponible pour un échange téléphonique cette semaine ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre restaurant Rajasthan et j'ai été impressionné par l'originalité de votre cuisine et l'ambiance chaleureuse que vous proposez à vos clients.
+Je pense que la création d'un reportage vidéo immersif sur votre activité pourrait vraiment mettre en valeur l'authenticité et la dynamique de votre établissement. De plus, une publicité courte et percutante pourrait renforcer votre présence en ligne et attirer de nouveaux clients.
+Une collaboration vidéo avec La Station vous permettrait de gagner en visibilité et de transmettre efficacement vos valeurs et votre passion pour la gastronomie indienne.
+Je vous propose un échange rapide pour discuter de vos besoins en matière de contenu vidéo et des possibilités de collaboration. Seriez-vous disponible pour un appel cette semaine ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Désinsectiseur 35 &amp; Apiculteur 35 cricrilabeille , ADP-s Apiculture Désinsectisation Piégeage services 35</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à la découverte de votre entreprise, Désinsectiseur 35 &amp; Apiculteur 35 ADP-s Apiculture Désinsectisation Piégeage services 35. Votre engagement en faveur de la biodiversité et de la protection des abeilles est admirable.
+J'ai visité votre site web et j'ai été impressionné par votre approche unique en tant qu'"Apiculteur &amp; Désinsectiseur", "Agriculteur &amp; Artisan". Votre vidéo promotionnelle actuelle est déjà très intéressante, mais je suis convaincu que nous pourrions collaborer pour créer des contenus vidéo encore plus percutants et engageants pour mettre en avant vos activités et vos valeurs.
+Je vous propose de discuter de la possibilité de réaliser un film d'entreprise mettant en lumière votre démarche écologique ou un reportage immersif sur vos activités de désinsectisation et d'apiculture. Une vidéo professionnelle pourrait renforcer votre visibilité, mettre en avant vos valeurs et renforcer votre crédibilité auprès de votre public cible.
+Si cette proposition suscite votre intérêt, je serais ravi de pouvoir échanger de vive voix pour discuter plus en détail de vos besoins et de nos services. Seriez-vous disponible pour un appel rapide cette semaine ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Arthur Bonnet - Cuisiniste Rennes - Melesse</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment visité votre site web et j'ai été impressionné par la qualité de vos produits et services. Votre expertise dans le domaine de la cuisine sur mesure est indéniable.
+Je me permets de vous contacter car je pense que la création de vidéos personnalisées pourrait grandement valoriser votre entreprise. En particulier, je vous propose un film d'entreprise mettant en avant votre savoir-faire et vos valeurs uniques. Cette vidéo pourrait renforcer votre visibilité en ligne et attirer de nouveaux clients en mettant en lumière ce qui vous distingue de vos concurrents.
+Je serais ravi de discuter plus en détail de cette opportunité et de voir comment La Station pourrait vous accompagner dans la réalisation de ce projet. Seriez-vous disponible pour un rendez-vous téléphonique rapide cette semaine ?
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Servagroupe Travail Temporaire Rennes</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Madame, Monsieur,
+Je me permets de vous contacter car je suis tombé sur votre site web et j'ai été impressionné par votre approche innovante dans le secteur du travail temporaire. Vos valeurs de qualité et d'engagement envers vos clients sont tout à fait louables.
+Je pense que la création d'un film d'entreprise mettant en avant vos collaborateurs et vos méthodes de travail pourrait être un excellent moyen de renforcer votre image de marque et de transmettre vos valeurs de manière authentique. De plus, un témoignage vidéo de vos clients satisfaits pourrait renforcer votre crédibilité et attirer de nouveaux partenaires.
+Si vous êtes intéressés par cette proposition, je serais ravi de discuter plus en détail de vos besoins et de voir comment La Station pourrait vous accompagner dans la réalisation de ces projets vidéo.
+Je vous propose un rendez-vous téléphonique rapide pour en discuter de vive voix. N'hésitez pas à me contacter par email ou par téléphone pour convenir d'un créneau qui vous conviendrait.
+Cordialement,
+Alan Roussel
+La Station
+contact@lastation-prod.com
+06 75 61 11 72
+www.lastation-prod.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>SEO - SOCIETE D'ETANCHEITE DE L'OUEST</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter au nom de l'agence La Station, spécialisée dans la création de vidéos personnalisées. En visitant votre site web, j'ai été impressionné par l'étendue de vos activités dans les secteurs des travaux publics et du bâtiment.
+Je pense que la réalisation d'un film d'entreprise mettant en avant vos réalisations et vos valeurs pourrait être un atout majeur pour votre communication. De plus, un témoignage vidéo de vos clients ou partenaires pourrait renforcer votre crédibilité et votre visibilité sur le marché.
+Nous serions ravis de pouvoir échanger avec vous sur la manière dont la vidéo peut contribuer à mettre en lumière votre expertise et vos engagements. 
+Souhaitez-vous convenir d'un rendez-vous téléphonique pour discuter de cette opportunité ?
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>NES COURTAGE</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre entreprise NES COURTAGE et je suis impressionné par votre engagement à accompagner les professionnels et les entreprises dans la gestion de leurs contrats d'assurance.
+Je suis Alan Roussel, expert en prospection B2B pour l'agence La Station, spécialisée dans la création de vidéos personnalisées. Nous pourrions envisager ensemble la réalisation d'un film d'entreprise mettant en lumière vos services et votre approche unique en matière d'assurance. Ce format vidéo pourrait renforcer votre visibilité en ligne et mettre en avant vos valeurs d'engagement et de réactivité.
+Je serais ravi de discuter plus en détail de cette opportunité lors d'un rendez-vous téléphonique rapide. N'hésitez pas à me contacter par email à contact@lastation-prod.com ou par téléphone au 06 75 61 11 72 pour convenir d'une date qui vous conviendrait.
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Bun Bol</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre restaurant Bun Bol et je suis impressionné par votre engagement à offrir une expérience culinaire vietnamienne authentique. Vos plats préparés avec soin et vos ingrédients frais témoignent de votre passion pour la culture vietnamienne.
+Je pense que la création de vidéos personnalisées pourrait mettre en lumière davantage vos plats et valeurs uniques. Un format de reportage immersif ou une publicité courte à fort impact pourraient véhiculer efficacement l'authenticité de votre cuisine et attirer de nouveaux clients en mettant en avant vos saveurs traditionnelles.
+Une collaboration vidéo avec La Station pourrait renforcer la visibilité de Bun Bol, mettre en avant vos valeurs et renforcer la crédibilité de votre établissement auprès de votre clientèle.
+Je serais ravi de discuter plus en détail de cette opportunité lors d'un rendez-vous rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>ACCOUNT REVISION</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à la découverte de votre entreprise, Account Revision. Votre expertise dans le domaine de la comptabilité et de la finance est indéniable, et je suis convaincu que la vidéo pourrait être un atout majeur pour mettre en avant vos services.
+Avez-vous déjà envisagé la réalisation d'un film d'entreprise mettant en lumière votre savoir-faire et vos valeurs ? Ou peut-être seriez-vous intéressés par des témoignages clients authentiques pour renforcer votre crédibilité ?
+La vidéo est un moyen puissant pour accroître votre visibilité, valoriser vos valeurs et renforcer votre image de marque. Chez La Station, nous sommes spécialisés dans la création de contenus vidéo originaux et impactants, et nous serions ravis de collaborer avec vous pour mettre en avant votre entreprise.
+Je vous propose un échange rapide pour discuter de vos besoins et des possibilités de collaboration. Seriez-vous disponible pour un rendez-vous téléphonique cette semaine ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Thélem assurances Rennes Jonathan TROCHEL</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à ma découverte de votre entreprise Thélem assurances à Rennes. Votre agence historique et votre approche centrée sur la satisfaction client m'ont particulièrement interpellé.
+Je constate que vous accordez une importance particulière à l'accompagnement de vos clients, et je suis convaincu que la création de contenus vidéo personnalisés pourrait renforcer encore davantage votre relation avec ces derniers. 
+Je vous propose ainsi de discuter de la possibilité de réaliser des vidéos de témoignages clients ou des reportages immersifs pour mettre en avant vos valeurs d'accueil et de proximité. Ces formats pourraient non seulement renforcer votre visibilité en ligne, mais aussi renforcer la crédibilité de votre agence.
+Je serais ravi de pouvoir échanger plus en détail sur ces opportunités lors d'un rendez-vous rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Ivisio 3D</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car je suis impressionné par votre approche innovante en matière de capture 3D et de visite virtuelle immersive. Votre site web est une véritable vitrine de vos réalisations exceptionnelles.
+Je pense que notre agence La Station pourrait vous aider à mettre en avant vos biens de manière encore plus percutante grâce à des vidéos personnalisées. En particulier, je vous propose de réaliser un reportage immersif pour mettre en valeur vos espaces de manière authentique et dynamique, ou une présentation produit pour analyser en détail les caractéristiques clés de vos biens.
+Une collaboration avec La Station vous permettrait de renforcer la visibilité de vos biens, d'exposer votre ambiance et votre originalité de manière unique, et de créer l'envie auprès de vos futurs clients de manière innovante.
+Je serais ravi de discuter de cette opportunité de collaboration lors d'un rendez-vous rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Styl Photo</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre entreprise, Styl Photo, et je suis impressionné par votre longue expérience dans le domaine de la photographie professionnelle. Votre studio et laboratoire équipés de matériel dernier cri semblent être un véritable atout pour vos clients.
+Je pense que notre agence, La Station, spécialisée dans la création de vidéos personnalisées, pourrait vous aider à mettre en avant votre savoir-faire et votre expertise à travers des formats vidéo adaptés à vos enjeux. Par exemple, un reportage immersif sur vos activités ou un aftermovie captivant des moments forts de vos séances photo pourraient renforcer votre visibilité et votre crédibilité auprès de votre audience.
+Je serais ravi de discuter plus en détail de la manière dont nous pourrions collaborer pour créer des contenus vidéo uniques et impactants pour Styl Photo. Seriez-vous disponible pour un appel rapide cette semaine afin d'échanger sur vos besoins et attentes en matière de communication visuelle ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Drone Air Flight</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre entreprise, Drone Air Flight, spécialisée dans les prises de vues aériennes et les photographies immobilières. Votre approche innovante et votre expertise dans ce domaine m'ont particulièrement impressionné.
+Je pense que la réalisation d'un film promotionnel ou d'une vidéo immersive pourrait grandement valoriser votre activité et mettre en lumière vos services uniques. Un reportage captivant sur vos interventions ou une publicité percutante mettant en avant vos compétences pourraient renforcer votre visibilité et votre crédibilité auprès de vos clients potentiels.
+Je serais ravi de discuter plus en détail de ces possibilités et de voir comment La Station pourrait vous accompagner dans la création de contenus vidéo originaux et impactants.
+Souhaitez-vous convenir d'un rendez-vous téléphonique rapide pour échanger plus en détail sur vos besoins et attentes en matière de communication visuelle ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Crazygrapherphoto Steve</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre site web Crazygrapherphoto Steve et j'ai été impressionné par votre approche authentique et passionnée de la photographie. Votre engagement à capturer des moments uniques et précieux est véritablement inspirant.
+Je pense que notre agence La Station pourrait vous aider à donner vie à vos histoires à travers des vidéos personnalisées. Nous pourrions par exemple collaborer sur la réalisation d'un reportage immersif pour mettre en lumière votre approche artistique ou d'une publicité percutante pour renforcer votre présence en ligne.
+Une vidéo professionnelle pourrait non seulement renforcer votre visibilité et votre crédibilité, mais aussi permettre à votre audience de mieux comprendre vos valeurs et votre passion pour la photographie.
+Je serais ravi de discuter plus en détail de la manière dont nous pourrions collaborer. Seriez-vous disponible pour un rendez-vous rapide cette semaine pour échanger plus en profondeur ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Céline Dufourd Photographie</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à la découverte de votre site web, http://www.celinedufourd.fr/. Votre approche artistique et votre sensibilité dans la photographie équine et canine sont remarquables.
+Je suis Alan Roussel, expert en prospection B2B pour l'agence La Station, spécialisée dans la création de vidéos personnalisées. Nous pourrions envisager de collaborer pour mettre en lumière la complicité entre les propriétaires et leurs animaux à travers des vidéos authentiques et artistiques.
+Je vous propose de discuter des formats vidéo tels que des reportages immersifs ou des présentations de produits mettant en valeur le caractère unique de chaque animal. Une vidéo personnalisée pourrait renforcer votre visibilité en ligne et souligner vos valeurs de respect et de passion pour les animaux.
+Si cette proposition suscite votre intérêt, je serais ravi d'échanger davantage lors d'un appel rapide pour discuter de vos besoins et attentes.
+Bien cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>AU BONHEUR PHOTO</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre site internet, et j'ai été impressionné par la qualité de vos photographies. Votre approche axée sur le photo-reportage pour capturer les émotions et les moments authentiques est tout à fait en phase avec notre expertise en création de vidéos personnalisées.
+Nous aimerions vous proposer la réalisation d'un reportage vidéo pour mettre en lumière votre travail et votre approche unique. Ce format permettrait de valoriser davantage la beauté et l'authenticité de vos clichés, tout en renforçant votre présence en ligne.
+De plus, nous pourrions également envisager la création d'une série de contenus pour les réseaux sociaux, afin de dynamiser votre communication et d'engager votre audience de manière plus interactive.
+Nous sommes convaincus que cette collaboration pourrait vous apporter une visibilité accrue et renforcer la crédibilité de votre entreprise auprès de votre clientèle.
+Serait-il possible de convenir d'un rendez-vous téléphonique rapide pour discuter plus en détail de ces opportunités de collaboration ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>waOh!</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Madame, Monsieur,
+Je me permets de vous contacter suite à la découverte de votre entreprise waOh! et de votre expertise en photos, vidéos et motions. Votre approche passionnée et complète en matière d'image m'a particulièrement interpellé.
+J'ai pu parcourir votre site web et j'ai été impressionné par la qualité de vos réalisations et par l'attention portée aux détails dans chacun de vos projets. Votre engagement pour satisfaire les envies visuelles de vos clients transparaît clairement.
+Je pense que notre agence La Station pourrait vous apporter une réelle valeur ajoutée en matière de vidéos personnalisées. Nous pourrions envisager ensemble la création d'un film d'entreprise mettant en lumière vos valeurs et votre savoir-faire, ou encore la réalisation d'un reportage captivant sur vos activités.
+Une collaboration avec La Station vous permettrait de renforcer votre visibilité, de valoriser vos produits et services, et de renforcer la crédibilité de votre entreprise auprès de votre audience.
+Je vous propose de convenir d'un rendez-vous rapide pour discuter plus en détail de vos besoins en matière de contenu vidéo et des possibilités de collaboration entre nos deux structures.
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel
+La Station
+contact@lastation-prod.com
+06 75 61 11 72
+www.lastation-prod.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Arnaud Vallée, Graphiste indépendant</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre site web et j'ai été impressionné par la qualité de vos créations graphiques. Votre travail témoigne d'une grande expertise et d'une réelle sensibilité artistique.
+Je pense que la réalisation d'une vidéo personnalisée pourrait mettre en lumière votre talent et vos réalisations de manière encore plus impactante. Un format de présentation de produit ou un aftermovie pour mettre en valeur vos créations pourraient véritablement renforcer votre visibilité et votre crédibilité auprès de votre audience.
+Je serais ravi de pouvoir échanger avec vous sur la possibilité d'une collaboration vidéo pour valoriser votre travail de manière dynamique et engageante. Seriez-vous disponible pour discuter de vos besoins et de vos attentes lors d'un rendez-vous rapide ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Agence Gosselin Design</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre entreprise, Agence Gosselin Design, et j'ai été impressionné par votre approche stratégique et créative en matière de communication et de design.
+Je me demandais comment vous envisagiez d'intégrer la vidéo dans votre stratégie globale. Avec notre expertise chez La Station, nous pourrions vous accompagner dans la création de vidéos personnalisées qui mettent en valeur votre marque et renforcent votre présence en ligne.
+Je pense notamment à la réalisation d'un film d'entreprise pour transmettre vos valeurs de manière authentique et engageante, ou à la création d'interviews de vos équipes pour humaniser votre communication. Ces formats pourraient vous permettre de gagner en visibilité et en crédibilité auprès de votre audience.
+Si cette proposition vous intéresse, je serais ravi de discuter plus en détail de vos besoins et de voir comment nous pourrions collaborer. Seriez-vous disponible pour un rendez-vous rapide cette semaine ?
+Bien cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>La Boîte à Pola - Location de photobooth/borne photo Rennes</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à la découverte de votre entreprise, La Boîte à Pola, spécialisée dans la location de photobooth à Rennes. Votre approche unique et créative pour offrir des souvenirs inoubliables lors d'événements festifs a retenu toute notre attention.
+Nous sommes l'agence La Station, basée à Rennes, spécialisée dans la création de vidéos personnalisées. Nous pensons que la mise en valeur de vos services à travers un film d'entreprise ou un reportage captivant pourrait renforcer votre visibilité et votre attractivité auprès de vos clients.
+Nous serions ravis de discuter avec vous des possibilités de collaboration pour créer des contenus vidéo originaux et impactants qui mettront en lumière l'expérience unique que vous proposez. 
+N'hésitez pas à me contacter pour convenir d'un rendez-vous ou d'un appel rapide afin d'échanger plus en détail sur votre projet.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Studio Faucher Photographies</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre entreprise, Studio Faucher Photographies, et j'ai été impressionné par la qualité de vos services et la passion que vous mettez dans la réalisation de vos photos.
+Je suis Alan Roussel, expert en prospection B2B pour l'agence La Station à Rennes, spécialisée dans la création de vidéos personnalisées. Nous travaillons avec des entreprises comme la vôtre pour mettre en lumière leur activité et leurs valeurs à travers des vidéos impactantes.
+Je suis convaincu que la vidéo pourrait être un excellent moyen de valoriser votre travail et de toucher un public plus large. Nous pourrions par exemple envisager la réalisation d'un reportage mettant en avant votre studio et votre approche unique, ou d'une vidéo de présentation de vos différents services pour renforcer votre visibilité en ligne.
+Une collaboration vidéo avec La Station pourrait vous permettre de renforcer votre image de marque, de gagner en crédibilité auprès de vos clients et de vous démarquer de la concurrence.
+Je serais ravi de pouvoir discuter plus en détail de ces possibilités lors d'un rendez-vous téléphonique rapide. N'hésitez pas à me contacter par email ou par téléphone pour convenir d'une date qui vous conviendrait.
+En espérant avoir l'opportunité de collaborer ensemble, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel
+La Station
+contact@lastation-prod.com
+06 75 61 11 72
+www.lastation-prod.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>MPhotographie Mélanie Maudieu</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre entreprise MPhotographie Mélanie Maudieu et j'ai été impressionné par votre présence en ligne sur votre page Facebook. Vos photos sont vraiment magnifiques et reflètent un réel talent pour la photographie.
+Je me permets de vous contacter car je pense que la vidéo pourrait être un excellent moyen de mettre en valeur votre travail et de toucher un public plus large. Je vous propose notamment la réalisation d'un reportage pour mettre en lumière votre activité et capturer l'authenticité de vos événements.
+En optant pour la vidéo, vous pourriez renforcer votre visibilité en ligne et transmettre vos valeurs de manière plus dynamique et engageante. Cela vous permettrait également de renforcer votre crédibilité auprès de vos clients et partenaires.
+Si cette proposition vous intéresse, je serais ravi de discuter plus en détail de vos besoins et de voir comment nous pourrions collaborer ensemble. Seriez-vous disponible pour un rendez-vous téléphonique rapide cette semaine ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Knecht Marc</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à ma découverte de votre site web. J'ai été impressionné par votre approche artistique et votre expertise dans le reportage d'événements d'entreprise.
+Je pense que la création d'un aftermovie de vos événements pourrait parfaitement mettre en valeur l'ambiance et l'authenticité de vos prestations. De plus, cela renforcerait votre visibilité en ligne et véhiculerait vos valeurs de manière dynamique et engageante.
+Serait-il possible d'échanger rapidement sur la possibilité d'une collaboration vidéo pour votre entreprise ? Je serais ravi de discuter de vos besoins spécifiques et de vous présenter nos services adaptés.
+Dans l'attente de votre retour, je vous propose de convenir d'un rendez-vous téléphonique ou d'une réunion en personne selon votre préférence.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>KevM Photo</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre site web et j'ai été impressionné par la qualité de vos photos sur https://kevmphoto.myportfolio.com/. Votre travail est vraiment remarquable !
+Je me permets de vous contacter car je pense que la vidéo pourrait être un excellent moyen de mettre en valeur votre talent et de toucher un public plus large. Nous pourrions envisager de réaliser un reportage immersif pour mettre en lumière votre processus de création ou une publicité percutante pour promouvoir vos services de manière originale.
+Une collaboration vidéo avec La Station pourrait vous offrir une visibilité accrue et renforcer votre crédibilité auprès de votre audience.
+Serait-il possible de discuter de cette opportunité lors d'un rendez-vous rapide ? Je suis convaincu que nous pourrions créer ensemble quelque chose de vraiment spécial.
+Bien cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Focus Naturel</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je suis Alan Roussel de l'agence La Station, spécialisée dans la création de vidéos personnalisées. En visitant votre site web, j'ai été impressionné par votre passion pour la nature et votre approche authentique de la photographie.
+Je pense que la vidéo pourrait être un excellent moyen de mettre en valeur votre travail et de partager votre vision avec un public plus large. Nous pourrions envisager de réaliser un reportage immersif sur votre activité ou une publicité percutante mettant en avant votre démarche artistique unique.
+Une collaboration vidéo avec La Station pourrait vous offrir une visibilité accrue, renforcer vos valeurs et crédibiliser votre démarche artistique. 
+Je serais ravi de discuter plus en détail de ces possibilités lors d'un rendez-vous téléphonique rapide. N'hésitez pas à me contacter pour convenir d'une date qui vous conviendrait.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ANIMAL ASSUR</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre site web Animal Assur et j'ai été impressionné par votre engagement envers la santé et le bien-être des animaux de compagnie. 
+Nous, à La Station, sommes spécialisés dans la création de vidéos personnalisées et impactantes pour les entreprises du secteur de l'assurance. Nous pensons que la vidéo pourrait être un excellent moyen de mettre en avant vos services et de renforcer la relation avec vos clients.
+Je vous propose de discuter des possibilités de collaboration pour la création d'un film d'entreprise mettant en avant vos valeurs et votre engagement envers les animaux. Nous pourrions également envisager la réalisation d'interviews de clients satisfaits pour renforcer la crédibilité de votre entreprise.
+Une vidéo bien réalisée pourrait non seulement augmenter votre visibilité en ligne, mais aussi renforcer la confiance de vos clients actuels et potentiels.
+Serait-il possible de convenir d'un rendez-vous téléphonique rapide pour discuter de cette opportunité plus en détail ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>SCP GRAIVE BRIZARD COMMISSAIRES DE JUSTICE (ex Huissiers de Justice)</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à ma découverte de votre entreprise SCP GRAIVE BRIZARD COMMISSAIRES DE JUSTICE. Votre site web est très informatif et met en avant votre expertise dans le domaine des huissiers de justice.
+Je pense que la création d'un film d'entreprise ou d'une interview pourrait être un excellent moyen de mettre en lumière votre savoir-faire et de renforcer votre crédibilité auprès de vos clients. Ces formats vidéo permettraient de valoriser vos services et de communiquer de manière authentique sur votre métier.
+Je serais ravi de pouvoir échanger avec vous sur les possibilités de collaboration et de discuter plus en détail de la manière dont La Station pourrait vous accompagner dans la réalisation de ces projets vidéo.
+Souhaitez-vous convenir d'un rendez-vous téléphonique pour en discuter de vive voix ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Les Tendances de Marlyse société M and Co design</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+J'ai récemment découvert votre entreprise, Les Tendances de Marlyse société M and Co design, et j'ai été impressionné par votre approche créative dans le domaine de l'architecture d'intérieur. Votre site web reflète parfaitement votre expertise et votre sens du design.
+Je pense que la création d'une vidéo personnalisée pourrait grandement valoriser votre travail et mettre en lumière vos projets uniques. Nous pourrions envisager un format de reportage pour mettre en avant vos réalisations et votre processus créatif, ou bien une vidéo de présentation de produit pour mettre en avant vos services de manière percutante.
+Une vidéo professionnelle pourrait renforcer votre visibilité en ligne, mettre en avant vos valeurs et renforcer votre crédibilité auprès de vos clients potentiels.
+Je serais ravi de discuter plus en détail de la manière dont La Station pourrait vous accompagner dans la création de contenus vidéo originaux et impactants. Seriez-vous disponible pour un rendez-vous rapide cette semaine pour en discuter ?
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>CL Courtage</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter car j'ai récemment découvert votre entreprise, CL Courtage, et je suis impressionné par votre expertise dans le domaine du courtage en prêt à Rennes.
+Je constate que vous accordez une importance particulière à l'accompagnement personnalisé de vos clients tout au long de leur projet. C'est pourquoi je pense qu'une collaboration avec notre agence La Station, spécialisée dans la création de vidéos personnalisées, pourrait vous permettre de mettre en avant cette approche unique et de renforcer votre visibilité.
+Je vous propose de discuter des possibilités de réalisation d'un film d'entreprise mettant en lumière vos services et vos valeurs, ou d'un témoignage client authentique qui renforcerait votre crédibilité auprès de votre audience.
+Cette vidéo pourrait être un véritable atout pour votre communication, en vous permettant de vous démarquer et de toucher votre cible de manière plus impactante.
+Je serais ravi de pouvoir échanger plus en détail sur ces idées et de vous présenter nos services. Seriez-vous disponible pour un rendez-vous téléphonique rapide cette semaine ?
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Eurovia Bretagne</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Madame, Monsieur,
+Je me permets de vous contacter suite à la découverte de vos récentes réalisations impressionnantes à Saint-Malo et Saint-Just. Votre expertise en rénovation urbaine et votre engagement dans des projets d'envergure sont véritablement inspirants.
+Dans le cadre de notre collaboration, je vous propose de mettre en lumière vos réalisations à travers un format de reportage captivant. Nous pourrions également envisager la création d'une vidéo de présentation de produit pour mettre en avant vos matériaux et techniques de qualité.
+Une vidéo professionnelle permettrait de valoriser votre savoir-faire, renforcer votre image de marque et accroître votre visibilité auprès de vos clients et partenaires.
+Souhaitez-vous échanger sur ces possibilités de collaboration ? Un appel rapide pourrait nous permettre de discuter plus en détail de vos besoins et attentes.
+Dans l'attente de votre retour, je vous souhaite une excellente journée.
+Cordialement,
+Alan Roussel  
+La Station  
+contact@lastation-prod.com  
+06 75 61 11 72  
+www.lastation-prod.com  </t>
         </is>
       </c>
     </row>

</xml_diff>